<commit_message>
Added in Header and fixed Load
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,6 +15,9 @@
     <sheet name="Database Schema" sheetId="1" r:id="rId1"/>
     <sheet name="Features" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Database Schema'!$A$26:$E$95</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -447,9 +450,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,6 +457,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,8 +1273,9 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="95" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1294,275 +1298,275 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="E4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="4"/>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-      <c r="E6" s="3" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="E7" s="3" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-      <c r="E8" s="3" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="E9" s="3" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="E10" s="3" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="E11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="E12" s="3" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="E13" s="3" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="E14" s="3" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="E15" s="3" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="E16" s="3" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="E17" s="3" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="E17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E30" s="3"/>
-      <c r="F30" s="4" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E31" s="3"/>
-      <c r="F31" s="4" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed game setup/transition to round 1
setupPlayers convert to players

only allow start if game selected and 2 or more players
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="107">
   <si>
     <t>Check one per group</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Rung-In-Late[</t>
+  </si>
+  <si>
+    <t>first:</t>
   </si>
 </sst>
 </file>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,6 +1122,9 @@
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>106</v>
+      </c>
       <c r="D64" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
Added in Game Check and Editable Help Input box
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Desktop\Jeopardy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Desktop\rogramming\Jeopardy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
   <si>
     <t>Check one per group</t>
   </si>
@@ -306,18 +306,12 @@
     <t>state:</t>
   </si>
   <si>
-    <t>lastLogin:</t>
-  </si>
-  <si>
     <t>//If ==0, advance</t>
   </si>
   <si>
     <t>!= to double1</t>
   </si>
   <si>
-    <t>//onLogin</t>
-  </si>
-  <si>
     <t>open:</t>
   </si>
   <si>
@@ -331,12 +325,6 @@
   </si>
   <si>
     <t>Partially filled games/categories</t>
-  </si>
-  <si>
-    <t>Session{</t>
-  </si>
-  <si>
-    <t>teamNumber:</t>
   </si>
   <si>
     <t>Incorrect[</t>
@@ -777,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +787,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,7 +981,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,7 +1063,7 @@
         <v>58</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -1115,15 +1103,15 @@
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D64" t="s">
         <v>86</v>
@@ -1131,7 +1119,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D65" t="s">
         <v>86</v>
@@ -1139,7 +1127,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D66" t="s">
         <v>85</v>
@@ -1155,14 +1143,6 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>92</v>
-      </c>
-      <c r="C69" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>31</v>
@@ -1186,7 +1166,7 @@
         <v>60</v>
       </c>
       <c r="D77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,7 +1189,7 @@
         <v>75</v>
       </c>
       <c r="E81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,21 +1241,6 @@
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1467,7 @@
     </row>
     <row r="21" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>7</v>
@@ -1558,7 +1523,7 @@
     </row>
     <row r="29" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="E29" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>13</v>

</xml_diff>